<commit_message>
add the step number of 05 March
</commit_message>
<xml_diff>
--- a/2017运动步数统计.xlsx
+++ b/2017运动步数统计.xlsx
@@ -442,7 +442,7 @@
   <dimension ref="A1:G366"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F123" sqref="F123"/>
+      <selection activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2939,6 +2939,9 @@
       </c>
       <c r="E123">
         <v>2</v>
+      </c>
+      <c r="F123">
+        <v>13807</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>